<commit_message>
Fix: Report "PCS" error
</commit_message>
<xml_diff>
--- a/Invoice/pur_inv.xlsx
+++ b/Invoice/pur_inv.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Invoice</t>
   </si>
@@ -78,18 +78,6 @@
     <t>natf0/6386</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Container</t>
-  </si>
-  <si>
-    <t>7x40`</t>
-  </si>
-  <si>
-    <t>4x40`</t>
-  </si>
-  <si>
     <t>Vessel</t>
   </si>
   <si>
@@ -97,6 +85,36 @@
   </si>
   <si>
     <t>ship-2</t>
+  </si>
+  <si>
+    <t>7x40'</t>
+  </si>
+  <si>
+    <t>4x40'</t>
+  </si>
+  <si>
+    <t>13X40'</t>
+  </si>
+  <si>
+    <t>natf0/6400</t>
+  </si>
+  <si>
+    <t>ship-3</t>
+  </si>
+  <si>
+    <t>cntnr-date</t>
+  </si>
+  <si>
+    <t>cntnr</t>
+  </si>
+  <si>
+    <t>02.02.2019</t>
+  </si>
+  <si>
+    <t>02.02.2020</t>
+  </si>
+  <si>
+    <t>02.02.2021</t>
   </si>
 </sst>
 </file>
@@ -593,11 +611,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -933,423 +952,493 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="11.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="14.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>23800</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>2100</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>9000</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1500</v>
       </c>
       <c r="H2" s="3">
         <v>1500</v>
       </c>
       <c r="I2" s="3">
+        <v>1500</v>
+      </c>
+      <c r="J2" s="3">
         <v>2200</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>1400</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>250</v>
       </c>
-      <c r="L2" s="3">
-        <v>0</v>
-      </c>
       <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
         <v>700</v>
       </c>
-      <c r="N2" s="3">
+      <c r="O2" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>23800</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>2100</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>9000</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1500</v>
       </c>
       <c r="H3" s="3">
         <v>1500</v>
       </c>
       <c r="I3" s="3">
+        <v>1500</v>
+      </c>
+      <c r="J3" s="3">
         <v>2200</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>1400</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>250</v>
       </c>
-      <c r="L3" s="3">
-        <v>0</v>
-      </c>
       <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
         <v>700</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3">
+        <v>28000</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2100</v>
+      </c>
+      <c r="G4" s="3">
+        <v>9000</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1350</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1250</v>
+      </c>
+      <c r="J4" s="3">
+        <v>950</v>
+      </c>
+      <c r="K4" s="3">
+        <v>600</v>
+      </c>
+      <c r="L4" s="3">
+        <v>100</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>300</v>
+      </c>
+      <c r="O4" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3">
+        <v>25200</v>
+      </c>
+      <c r="F5" s="3">
+        <v>900</v>
+      </c>
+      <c r="G5" s="3">
+        <v>8450</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3300</v>
+      </c>
+      <c r="I5" s="3">
+        <v>500</v>
+      </c>
+      <c r="J5" s="3">
+        <v>5450</v>
+      </c>
+      <c r="K5" s="3">
+        <v>3250</v>
+      </c>
+      <c r="L5" s="3">
+        <v>50</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>600</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3">
+        <v>26900</v>
+      </c>
+      <c r="F6" s="3">
+        <v>900</v>
+      </c>
+      <c r="G6" s="3">
+        <v>7350</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2900</v>
+      </c>
+      <c r="I6" s="3">
+        <v>450</v>
+      </c>
+      <c r="J6" s="3">
+        <v>5000</v>
+      </c>
+      <c r="K6" s="3">
+        <v>3000</v>
+      </c>
+      <c r="L6" s="3">
+        <v>100</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>550</v>
+      </c>
+      <c r="O6" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3">
+        <v>25200</v>
+      </c>
+      <c r="F7" s="3">
+        <v>900</v>
+      </c>
+      <c r="G7" s="3">
+        <v>8450</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3300</v>
+      </c>
+      <c r="I7" s="3">
+        <v>500</v>
+      </c>
+      <c r="J7" s="3">
+        <v>5450</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3250</v>
+      </c>
+      <c r="L7" s="3">
+        <v>50</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>600</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3">
+        <v>25200</v>
+      </c>
+      <c r="F8" s="3">
+        <v>900</v>
+      </c>
+      <c r="G8" s="3">
+        <v>8450</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3300</v>
+      </c>
+      <c r="I8" s="3">
+        <v>500</v>
+      </c>
+      <c r="J8" s="3">
+        <v>5450</v>
+      </c>
+      <c r="K8" s="3">
+        <v>3250</v>
+      </c>
+      <c r="L8" s="3">
+        <v>50</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>600</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="3">
+        <v>104000</v>
+      </c>
+      <c r="F9" s="3">
+        <v>5800</v>
+      </c>
+      <c r="G9" s="3">
+        <v>18000</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5000</v>
+      </c>
+      <c r="I9" s="3">
+        <v>2500</v>
+      </c>
+      <c r="J9" s="3">
+        <v>12600</v>
+      </c>
+      <c r="K9" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L9" s="3">
+        <v>600</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>100</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3">
-        <v>28000</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2100</v>
-      </c>
-      <c r="F4" s="3">
-        <v>9000</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1350</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1250</v>
-      </c>
-      <c r="I4" s="3">
+      <c r="D10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3">
+        <v>351800</v>
+      </c>
+      <c r="F10" s="3">
+        <v>7900</v>
+      </c>
+      <c r="G10" s="3">
+        <v>51600</v>
+      </c>
+      <c r="H10" s="3">
+        <v>18750</v>
+      </c>
+      <c r="I10" s="3">
+        <v>3550</v>
+      </c>
+      <c r="J10" s="3">
+        <v>38000</v>
+      </c>
+      <c r="K10" s="3">
+        <v>20450</v>
+      </c>
+      <c r="L10" s="3">
         <v>950</v>
       </c>
-      <c r="J4" s="3">
-        <v>600</v>
-      </c>
-      <c r="K4" s="3">
-        <v>100</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>300</v>
-      </c>
-      <c r="N4" s="3">
-        <v>50</v>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <v>2050</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3">
-        <v>25200</v>
-      </c>
-      <c r="E5" s="3">
-        <v>900</v>
-      </c>
-      <c r="F5" s="3">
-        <v>8450</v>
-      </c>
-      <c r="G5" s="3">
-        <v>3300</v>
-      </c>
-      <c r="H5" s="3">
-        <v>500</v>
-      </c>
-      <c r="I5" s="3">
-        <v>5450</v>
-      </c>
-      <c r="J5" s="3">
-        <v>3250</v>
-      </c>
-      <c r="K5" s="3">
-        <v>50</v>
-      </c>
-      <c r="L5" s="3">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
-        <v>600</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3">
-        <v>26900</v>
-      </c>
-      <c r="E6" s="3">
-        <v>900</v>
-      </c>
-      <c r="F6" s="3">
-        <v>7350</v>
-      </c>
-      <c r="G6" s="3">
-        <v>2900</v>
-      </c>
-      <c r="H6" s="3">
-        <v>450</v>
-      </c>
-      <c r="I6" s="3">
-        <v>5000</v>
-      </c>
-      <c r="J6" s="3">
-        <v>3000</v>
-      </c>
-      <c r="K6" s="3">
-        <v>100</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>550</v>
-      </c>
-      <c r="N6" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3">
-        <v>25200</v>
-      </c>
-      <c r="E7" s="3">
-        <v>900</v>
-      </c>
-      <c r="F7" s="3">
-        <v>8450</v>
-      </c>
-      <c r="G7" s="3">
-        <v>3300</v>
-      </c>
-      <c r="H7" s="3">
-        <v>500</v>
-      </c>
-      <c r="I7" s="3">
-        <v>5450</v>
-      </c>
-      <c r="J7" s="3">
-        <v>3250</v>
-      </c>
-      <c r="K7" s="3">
-        <v>50</v>
-      </c>
-      <c r="L7" s="3">
-        <v>0</v>
-      </c>
-      <c r="M7" s="3">
-        <v>600</v>
-      </c>
-      <c r="N7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="3">
-        <v>25200</v>
-      </c>
-      <c r="E8" s="3">
-        <v>900</v>
-      </c>
-      <c r="F8" s="3">
-        <v>8450</v>
-      </c>
-      <c r="G8" s="3">
-        <v>3300</v>
-      </c>
-      <c r="H8" s="3">
-        <v>500</v>
-      </c>
-      <c r="I8" s="3">
-        <v>5450</v>
-      </c>
-      <c r="J8" s="3">
-        <v>3250</v>
-      </c>
-      <c r="K8" s="3">
-        <v>50</v>
-      </c>
-      <c r="L8" s="3">
-        <v>0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>600</v>
-      </c>
-      <c r="N8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3">
-        <v>104000</v>
-      </c>
-      <c r="E9" s="3">
-        <v>5800</v>
-      </c>
-      <c r="F9" s="3">
-        <v>18000</v>
-      </c>
-      <c r="G9" s="3">
-        <v>5000</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2500</v>
-      </c>
-      <c r="I9" s="3">
-        <v>12600</v>
-      </c>
-      <c r="J9" s="3">
-        <v>10000</v>
-      </c>
-      <c r="K9" s="3">
-        <v>600</v>
-      </c>
-      <c r="L9" s="3">
-        <v>0</v>
-      </c>
-      <c r="M9" s="3">
-        <v>100</v>
-      </c>
-      <c r="N9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4">
-      <c r="D18" s="1"/>
+    <row r="18" spans="5:5">
+      <c r="E18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added: Ship Wise Invoice
</commit_message>
<xml_diff>
--- a/Invoice/pur_inv.xlsx
+++ b/Invoice/pur_inv.xlsx
@@ -16,43 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
-  <si>
-    <t>Invoice</t>
-  </si>
-  <si>
-    <t>8x4</t>
-  </si>
-  <si>
-    <t>8x3</t>
-  </si>
-  <si>
-    <t>7x4</t>
-  </si>
-  <si>
-    <t>7x3</t>
-  </si>
-  <si>
-    <t>7x2.5</t>
-  </si>
-  <si>
-    <t>6x4</t>
-  </si>
-  <si>
-    <t>6x3</t>
-  </si>
-  <si>
-    <t>6x2.5</t>
-  </si>
-  <si>
-    <t>5x4</t>
-  </si>
-  <si>
-    <t>5x3</t>
-  </si>
-  <si>
-    <t>5x2.5</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>f-001</t>
   </si>
@@ -102,12 +66,6 @@
     <t>ship-3</t>
   </si>
   <si>
-    <t>cntnr-date</t>
-  </si>
-  <si>
-    <t>Container</t>
-  </si>
-  <si>
     <t>15.01.2021</t>
   </si>
   <si>
@@ -126,7 +84,88 @@
     <t>31.01.2021</t>
   </si>
   <si>
-    <t>INV_ID</t>
+    <t>8X4</t>
+  </si>
+  <si>
+    <t>8X3</t>
+  </si>
+  <si>
+    <t>7X4</t>
+  </si>
+  <si>
+    <t>7X3</t>
+  </si>
+  <si>
+    <t>7X2.5</t>
+  </si>
+  <si>
+    <t>6X4</t>
+  </si>
+  <si>
+    <t>6X3</t>
+  </si>
+  <si>
+    <t>6X2.5</t>
+  </si>
+  <si>
+    <t>5X4</t>
+  </si>
+  <si>
+    <t>5X3</t>
+  </si>
+  <si>
+    <t>5X2.5</t>
+  </si>
+  <si>
+    <t>SHIP_ID</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>i1</t>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>i3</t>
+  </si>
+  <si>
+    <t>i4</t>
+  </si>
+  <si>
+    <t>i5</t>
+  </si>
+  <si>
+    <t>i6</t>
+  </si>
+  <si>
+    <t>i7</t>
+  </si>
+  <si>
+    <t>i8</t>
+  </si>
+  <si>
+    <t>i9</t>
+  </si>
+  <si>
+    <t>PUR_INV_ID</t>
+  </si>
+  <si>
+    <t>Cntnr_date</t>
+  </si>
+  <si>
+    <t>INVOICE NO</t>
+  </si>
+  <si>
+    <t>CNTNR NO</t>
   </si>
 </sst>
 </file>
@@ -964,523 +1003,554 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="14.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="12.140625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="14.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
         <v>23800</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>2100</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>9000</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1500</v>
       </c>
       <c r="J2" s="3">
         <v>1500</v>
       </c>
       <c r="K2" s="3">
+        <v>1500</v>
+      </c>
+      <c r="L2" s="3">
         <v>2200</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>1400</v>
       </c>
-      <c r="M2" s="3">
+      <c r="N2" s="3">
         <v>250</v>
       </c>
-      <c r="N2" s="3">
-        <v>0</v>
-      </c>
       <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
         <v>700</v>
       </c>
-      <c r="P2" s="3">
+      <c r="Q2" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="2">
+    <row r="3" spans="1:17">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>23800</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>2100</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>9000</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1500</v>
       </c>
       <c r="J3" s="3">
         <v>1500</v>
       </c>
       <c r="K3" s="3">
+        <v>1500</v>
+      </c>
+      <c r="L3" s="3">
         <v>2200</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
         <v>1400</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>250</v>
       </c>
-      <c r="N3" s="3">
-        <v>0</v>
-      </c>
       <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
         <v>700</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="2">
+    <row r="4" spans="1:17">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="G4" s="3">
+        <v>28000</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2100</v>
+      </c>
+      <c r="I4" s="3">
+        <v>9000</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1350</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1250</v>
+      </c>
+      <c r="L4" s="3">
+        <v>950</v>
+      </c>
+      <c r="M4" s="3">
+        <v>600</v>
+      </c>
+      <c r="N4" s="3">
+        <v>100</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>300</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3">
+        <v>25200</v>
+      </c>
+      <c r="H5" s="3">
+        <v>900</v>
+      </c>
+      <c r="I5" s="3">
+        <v>8450</v>
+      </c>
+      <c r="J5" s="3">
+        <v>3300</v>
+      </c>
+      <c r="K5" s="3">
+        <v>500</v>
+      </c>
+      <c r="L5" s="3">
+        <v>5450</v>
+      </c>
+      <c r="M5" s="3">
+        <v>3250</v>
+      </c>
+      <c r="N5" s="3">
+        <v>50</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>600</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>26900</v>
+      </c>
+      <c r="H6" s="3">
+        <v>900</v>
+      </c>
+      <c r="I6" s="3">
+        <v>7350</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2900</v>
+      </c>
+      <c r="K6" s="3">
+        <v>450</v>
+      </c>
+      <c r="L6" s="3">
+        <v>5000</v>
+      </c>
+      <c r="M6" s="3">
+        <v>3000</v>
+      </c>
+      <c r="N6" s="3">
+        <v>100</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>550</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>25200</v>
+      </c>
+      <c r="H7" s="3">
+        <v>900</v>
+      </c>
+      <c r="I7" s="3">
+        <v>8450</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3300</v>
+      </c>
+      <c r="K7" s="3">
+        <v>500</v>
+      </c>
+      <c r="L7" s="3">
+        <v>5450</v>
+      </c>
+      <c r="M7" s="3">
+        <v>3250</v>
+      </c>
+      <c r="N7" s="3">
+        <v>50</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>600</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="3">
+        <v>25200</v>
+      </c>
+      <c r="H8" s="3">
+        <v>900</v>
+      </c>
+      <c r="I8" s="3">
+        <v>8450</v>
+      </c>
+      <c r="J8" s="3">
+        <v>3300</v>
+      </c>
+      <c r="K8" s="3">
+        <v>500</v>
+      </c>
+      <c r="L8" s="3">
+        <v>5450</v>
+      </c>
+      <c r="M8" s="3">
+        <v>3250</v>
+      </c>
+      <c r="N8" s="3">
+        <v>50</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>600</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="3">
+        <v>104000</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5800</v>
+      </c>
+      <c r="I9" s="3">
+        <v>18000</v>
+      </c>
+      <c r="J9" s="3">
+        <v>5000</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2500</v>
+      </c>
+      <c r="L9" s="3">
+        <v>12600</v>
+      </c>
+      <c r="M9" s="3">
+        <v>10000</v>
+      </c>
+      <c r="N9" s="3">
+        <v>600</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>100</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="E10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="3">
-        <v>28000</v>
-      </c>
-      <c r="G4" s="3">
-        <v>2100</v>
-      </c>
-      <c r="H4" s="3">
-        <v>9000</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1350</v>
-      </c>
-      <c r="J4" s="3">
-        <v>1250</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="G10" s="3">
+        <v>351800</v>
+      </c>
+      <c r="H10" s="3">
+        <v>7900</v>
+      </c>
+      <c r="I10" s="3">
+        <v>51600</v>
+      </c>
+      <c r="J10" s="3">
+        <v>18750</v>
+      </c>
+      <c r="K10" s="3">
+        <v>3550</v>
+      </c>
+      <c r="L10" s="3">
+        <v>38000</v>
+      </c>
+      <c r="M10" s="3">
+        <v>20450</v>
+      </c>
+      <c r="N10" s="3">
         <v>950</v>
       </c>
-      <c r="L4" s="3">
-        <v>600</v>
-      </c>
-      <c r="M4" s="3">
-        <v>100</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
-        <v>300</v>
-      </c>
-      <c r="P4" s="3">
-        <v>50</v>
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3">
+        <v>2050</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="3">
-        <v>25200</v>
-      </c>
-      <c r="G5" s="3">
-        <v>900</v>
-      </c>
-      <c r="H5" s="3">
-        <v>8450</v>
-      </c>
-      <c r="I5" s="3">
-        <v>3300</v>
-      </c>
-      <c r="J5" s="3">
-        <v>500</v>
-      </c>
-      <c r="K5" s="3">
-        <v>5450</v>
-      </c>
-      <c r="L5" s="3">
-        <v>3250</v>
-      </c>
-      <c r="M5" s="3">
-        <v>50</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
-        <v>600</v>
-      </c>
-      <c r="P5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3">
-        <v>26900</v>
-      </c>
-      <c r="G6" s="3">
-        <v>900</v>
-      </c>
-      <c r="H6" s="3">
-        <v>7350</v>
-      </c>
-      <c r="I6" s="3">
-        <v>2900</v>
-      </c>
-      <c r="J6" s="3">
-        <v>450</v>
-      </c>
-      <c r="K6" s="3">
-        <v>5000</v>
-      </c>
-      <c r="L6" s="3">
-        <v>3000</v>
-      </c>
-      <c r="M6" s="3">
-        <v>100</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>550</v>
-      </c>
-      <c r="P6" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="3">
-        <v>25200</v>
-      </c>
-      <c r="G7" s="3">
-        <v>900</v>
-      </c>
-      <c r="H7" s="3">
-        <v>8450</v>
-      </c>
-      <c r="I7" s="3">
-        <v>3300</v>
-      </c>
-      <c r="J7" s="3">
-        <v>500</v>
-      </c>
-      <c r="K7" s="3">
-        <v>5450</v>
-      </c>
-      <c r="L7" s="3">
-        <v>3250</v>
-      </c>
-      <c r="M7" s="3">
-        <v>50</v>
-      </c>
-      <c r="N7" s="3">
-        <v>0</v>
-      </c>
-      <c r="O7" s="3">
-        <v>600</v>
-      </c>
-      <c r="P7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="3">
-        <v>25200</v>
-      </c>
-      <c r="G8" s="3">
-        <v>900</v>
-      </c>
-      <c r="H8" s="3">
-        <v>8450</v>
-      </c>
-      <c r="I8" s="3">
-        <v>3300</v>
-      </c>
-      <c r="J8" s="3">
-        <v>500</v>
-      </c>
-      <c r="K8" s="3">
-        <v>5450</v>
-      </c>
-      <c r="L8" s="3">
-        <v>3250</v>
-      </c>
-      <c r="M8" s="3">
-        <v>50</v>
-      </c>
-      <c r="N8" s="3">
-        <v>0</v>
-      </c>
-      <c r="O8" s="3">
-        <v>600</v>
-      </c>
-      <c r="P8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="3">
-        <v>104000</v>
-      </c>
-      <c r="G9" s="3">
-        <v>5800</v>
-      </c>
-      <c r="H9" s="3">
-        <v>18000</v>
-      </c>
-      <c r="I9" s="3">
-        <v>5000</v>
-      </c>
-      <c r="J9" s="3">
-        <v>2500</v>
-      </c>
-      <c r="K9" s="3">
-        <v>12600</v>
-      </c>
-      <c r="L9" s="3">
-        <v>10000</v>
-      </c>
-      <c r="M9" s="3">
-        <v>600</v>
-      </c>
-      <c r="N9" s="3">
-        <v>0</v>
-      </c>
-      <c r="O9" s="3">
-        <v>100</v>
-      </c>
-      <c r="P9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="3">
-        <v>351800</v>
-      </c>
-      <c r="G10" s="3">
-        <v>7900</v>
-      </c>
-      <c r="H10" s="3">
-        <v>51600</v>
-      </c>
-      <c r="I10" s="3">
-        <v>18750</v>
-      </c>
-      <c r="J10" s="3">
-        <v>3550</v>
-      </c>
-      <c r="K10" s="3">
-        <v>38000</v>
-      </c>
-      <c r="L10" s="3">
-        <v>20450</v>
-      </c>
-      <c r="M10" s="3">
-        <v>950</v>
-      </c>
-      <c r="N10" s="3">
-        <v>0</v>
-      </c>
-      <c r="O10" s="3">
-        <v>2050</v>
-      </c>
-      <c r="P10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6">
-      <c r="F18" s="1"/>
+    <row r="18" spans="7:7">
+      <c r="G18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix: PUR_INV_ID key error
</commit_message>
<xml_diff>
--- a/Invoice/pur_inv.xlsx
+++ b/Invoice/pur_inv.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
   <si>
     <t>f-001</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Vessel</t>
   </si>
   <si>
-    <t>ship-1</t>
-  </si>
-  <si>
-    <t>ship-2</t>
-  </si>
-  <si>
     <t>7x40'</t>
   </si>
   <si>
@@ -63,27 +57,6 @@
     <t>natf0/6400</t>
   </si>
   <si>
-    <t>ship-3</t>
-  </si>
-  <si>
-    <t>15.01.2021</t>
-  </si>
-  <si>
-    <t>16.01.2021</t>
-  </si>
-  <si>
-    <t>17.01.2021</t>
-  </si>
-  <si>
-    <t>19.01.2021</t>
-  </si>
-  <si>
-    <t>30.01.2021</t>
-  </si>
-  <si>
-    <t>31.01.2021</t>
-  </si>
-  <si>
     <t>8X4</t>
   </si>
   <si>
@@ -166,6 +139,84 @@
   </si>
   <si>
     <t>CNTNR NO</t>
+  </si>
+  <si>
+    <t>Inv date</t>
+  </si>
+  <si>
+    <t>04.07.20</t>
+  </si>
+  <si>
+    <t>05.07.20</t>
+  </si>
+  <si>
+    <t>06.07.20</t>
+  </si>
+  <si>
+    <t>07.07.20</t>
+  </si>
+  <si>
+    <t>08.07.20</t>
+  </si>
+  <si>
+    <t>29.05.20</t>
+  </si>
+  <si>
+    <t>29.10.20</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Kanyin Face veneer</t>
+  </si>
+  <si>
+    <t>s4</t>
+  </si>
+  <si>
+    <t>i10</t>
+  </si>
+  <si>
+    <t>Sinar Solo</t>
+  </si>
+  <si>
+    <t>05.01.21</t>
+  </si>
+  <si>
+    <t>4X40'</t>
+  </si>
+  <si>
+    <t>WBL/136</t>
+  </si>
+  <si>
+    <t>05.07.2020</t>
+  </si>
+  <si>
+    <t>06.07.2020</t>
+  </si>
+  <si>
+    <t>07.07.2020</t>
+  </si>
+  <si>
+    <t>08.07.2020</t>
+  </si>
+  <si>
+    <t>09.07.2020</t>
+  </si>
+  <si>
+    <t>Kuo Hsiung(VZG)</t>
+  </si>
+  <si>
+    <t>21.07.2020</t>
+  </si>
+  <si>
+    <t>05.12.2020</t>
+  </si>
+  <si>
+    <t>Yantra Bhum(MLR)</t>
+  </si>
+  <si>
+    <t>Taloja(COCHIN)</t>
   </si>
 </sst>
 </file>
@@ -1003,554 +1054,672 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="14.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="11" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="3">
+        <v>23800</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2100</v>
+      </c>
+      <c r="K2" s="3">
+        <v>9000</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1500</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1500</v>
+      </c>
+      <c r="N2" s="3">
+        <v>2200</v>
+      </c>
+      <c r="O2" s="3">
+        <v>1400</v>
+      </c>
+      <c r="P2" s="3">
+        <v>250</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0</v>
+      </c>
+      <c r="R2" s="3">
+        <v>700</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>23800</v>
-      </c>
-      <c r="H2" s="3">
-        <v>2100</v>
-      </c>
-      <c r="I2" s="3">
-        <v>9000</v>
-      </c>
-      <c r="J2" s="3">
-        <v>1500</v>
-      </c>
-      <c r="K2" s="3">
-        <v>1500</v>
-      </c>
-      <c r="L2" s="3">
-        <v>2200</v>
-      </c>
-      <c r="M2" s="3">
-        <v>1400</v>
-      </c>
-      <c r="N2" s="3">
-        <v>250</v>
-      </c>
-      <c r="O2" s="3">
-        <v>0</v>
-      </c>
-      <c r="P2" s="3">
-        <v>700</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="3">
         <v>23800</v>
       </c>
-      <c r="H3" s="3">
+      <c r="J3" s="3">
         <v>2100</v>
       </c>
-      <c r="I3" s="3">
+      <c r="K3" s="3">
         <v>9000</v>
       </c>
-      <c r="J3" s="3">
+      <c r="L3" s="3">
         <v>1500</v>
       </c>
-      <c r="K3" s="3">
+      <c r="M3" s="3">
         <v>1500</v>
       </c>
-      <c r="L3" s="3">
+      <c r="N3" s="3">
         <v>2200</v>
       </c>
-      <c r="M3" s="3">
+      <c r="O3" s="3">
         <v>1400</v>
       </c>
-      <c r="N3" s="3">
+      <c r="P3" s="3">
         <v>250</v>
       </c>
-      <c r="O3" s="3">
-        <v>0</v>
-      </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3">
         <v>700</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="S3" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:19">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3">
         <v>28000</v>
       </c>
-      <c r="H4" s="3">
+      <c r="J4" s="3">
         <v>2100</v>
       </c>
-      <c r="I4" s="3">
+      <c r="K4" s="3">
         <v>9000</v>
       </c>
-      <c r="J4" s="3">
+      <c r="L4" s="3">
         <v>1350</v>
       </c>
-      <c r="K4" s="3">
+      <c r="M4" s="3">
         <v>1250</v>
       </c>
-      <c r="L4" s="3">
+      <c r="N4" s="3">
         <v>950</v>
       </c>
-      <c r="M4" s="3">
+      <c r="O4" s="3">
         <v>600</v>
       </c>
-      <c r="N4" s="3">
+      <c r="P4" s="3">
         <v>100</v>
       </c>
-      <c r="O4" s="3">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3">
         <v>300</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="S4" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:19">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="3">
         <v>25200</v>
       </c>
-      <c r="H5" s="3">
+      <c r="J5" s="3">
         <v>900</v>
       </c>
-      <c r="I5" s="3">
+      <c r="K5" s="3">
         <v>8450</v>
       </c>
-      <c r="J5" s="3">
+      <c r="L5" s="3">
         <v>3300</v>
       </c>
-      <c r="K5" s="3">
+      <c r="M5" s="3">
         <v>500</v>
       </c>
-      <c r="L5" s="3">
+      <c r="N5" s="3">
         <v>5450</v>
       </c>
-      <c r="M5" s="3">
+      <c r="O5" s="3">
         <v>3250</v>
       </c>
-      <c r="N5" s="3">
+      <c r="P5" s="3">
         <v>50</v>
       </c>
-      <c r="O5" s="3">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3">
+      <c r="Q5" s="3">
+        <v>0</v>
+      </c>
+      <c r="R5" s="3">
         <v>600</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="S5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:19">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="3">
         <v>26900</v>
       </c>
-      <c r="H6" s="3">
+      <c r="J6" s="3">
         <v>900</v>
       </c>
-      <c r="I6" s="3">
+      <c r="K6" s="3">
         <v>7350</v>
       </c>
-      <c r="J6" s="3">
+      <c r="L6" s="3">
         <v>2900</v>
       </c>
-      <c r="K6" s="3">
+      <c r="M6" s="3">
         <v>450</v>
       </c>
-      <c r="L6" s="3">
+      <c r="N6" s="3">
         <v>5000</v>
       </c>
-      <c r="M6" s="3">
+      <c r="O6" s="3">
         <v>3000</v>
       </c>
-      <c r="N6" s="3">
+      <c r="P6" s="3">
         <v>100</v>
       </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3">
         <v>550</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="S6" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:19">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="3">
         <v>25200</v>
       </c>
-      <c r="H7" s="3">
+      <c r="J7" s="3">
         <v>900</v>
       </c>
-      <c r="I7" s="3">
+      <c r="K7" s="3">
         <v>8450</v>
       </c>
-      <c r="J7" s="3">
+      <c r="L7" s="3">
         <v>3300</v>
       </c>
-      <c r="K7" s="3">
+      <c r="M7" s="3">
         <v>500</v>
       </c>
-      <c r="L7" s="3">
+      <c r="N7" s="3">
         <v>5450</v>
       </c>
-      <c r="M7" s="3">
+      <c r="O7" s="3">
         <v>3250</v>
       </c>
-      <c r="N7" s="3">
+      <c r="P7" s="3">
         <v>50</v>
       </c>
-      <c r="O7" s="3">
-        <v>0</v>
-      </c>
-      <c r="P7" s="3">
+      <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3">
         <v>600</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="S7" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:19">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="3">
         <v>25200</v>
       </c>
-      <c r="H8" s="3">
+      <c r="J8" s="3">
         <v>900</v>
       </c>
-      <c r="I8" s="3">
+      <c r="K8" s="3">
         <v>8450</v>
       </c>
-      <c r="J8" s="3">
+      <c r="L8" s="3">
         <v>3300</v>
       </c>
-      <c r="K8" s="3">
+      <c r="M8" s="3">
         <v>500</v>
       </c>
-      <c r="L8" s="3">
+      <c r="N8" s="3">
         <v>5450</v>
       </c>
-      <c r="M8" s="3">
+      <c r="O8" s="3">
         <v>3250</v>
       </c>
-      <c r="N8" s="3">
+      <c r="P8" s="3">
         <v>50</v>
       </c>
-      <c r="O8" s="3">
-        <v>0</v>
-      </c>
-      <c r="P8" s="3">
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3">
         <v>600</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="S8" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:19">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="3">
         <v>104000</v>
       </c>
-      <c r="H9" s="3">
+      <c r="J9" s="3">
         <v>5800</v>
       </c>
-      <c r="I9" s="3">
+      <c r="K9" s="3">
         <v>18000</v>
       </c>
-      <c r="J9" s="3">
+      <c r="L9" s="3">
         <v>5000</v>
       </c>
-      <c r="K9" s="3">
+      <c r="M9" s="3">
         <v>2500</v>
       </c>
-      <c r="L9" s="3">
+      <c r="N9" s="3">
         <v>12600</v>
       </c>
-      <c r="M9" s="3">
+      <c r="O9" s="3">
         <v>10000</v>
       </c>
-      <c r="N9" s="3">
+      <c r="P9" s="3">
         <v>600</v>
       </c>
-      <c r="O9" s="3">
-        <v>0</v>
-      </c>
-      <c r="P9" s="3">
+      <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
         <v>100</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="S9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:19">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="3">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="3">
         <v>351800</v>
       </c>
-      <c r="H10" s="3">
+      <c r="J10" s="3">
         <v>7900</v>
       </c>
-      <c r="I10" s="3">
+      <c r="K10" s="3">
         <v>51600</v>
       </c>
-      <c r="J10" s="3">
+      <c r="L10" s="3">
         <v>18750</v>
       </c>
-      <c r="K10" s="3">
+      <c r="M10" s="3">
         <v>3550</v>
       </c>
-      <c r="L10" s="3">
+      <c r="N10" s="3">
         <v>38000</v>
       </c>
-      <c r="M10" s="3">
+      <c r="O10" s="3">
         <v>20450</v>
       </c>
-      <c r="N10" s="3">
+      <c r="P10" s="3">
         <v>950</v>
       </c>
-      <c r="O10" s="3">
-        <v>0</v>
-      </c>
-      <c r="P10" s="3">
+      <c r="Q10" s="3">
+        <v>0</v>
+      </c>
+      <c r="R10" s="3">
         <v>2050</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="S10" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="7:7">
-      <c r="G18" s="1"/>
+    <row r="11" spans="1:19">
+      <c r="A11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="2">
+        <v>109100</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2800</v>
+      </c>
+      <c r="K11" s="2">
+        <v>18900</v>
+      </c>
+      <c r="L11" s="2">
+        <v>5200</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1500</v>
+      </c>
+      <c r="N11" s="2">
+        <v>13100</v>
+      </c>
+      <c r="O11" s="2">
+        <v>6700</v>
+      </c>
+      <c r="P11" s="2">
+        <v>150</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>1550</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9">
+      <c r="I18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added: opening and closing bal of pur_inv
</commit_message>
<xml_diff>
--- a/Invoice/pur_inv.xlsx
+++ b/Invoice/pur_inv.xlsx
@@ -93,42 +93,6 @@
     <t>SHIP_ID</t>
   </si>
   <si>
-    <t>s1</t>
-  </si>
-  <si>
-    <t>s2</t>
-  </si>
-  <si>
-    <t>s3</t>
-  </si>
-  <si>
-    <t>i1</t>
-  </si>
-  <si>
-    <t>i2</t>
-  </si>
-  <si>
-    <t>i3</t>
-  </si>
-  <si>
-    <t>i4</t>
-  </si>
-  <si>
-    <t>i5</t>
-  </si>
-  <si>
-    <t>i6</t>
-  </si>
-  <si>
-    <t>i7</t>
-  </si>
-  <si>
-    <t>i8</t>
-  </si>
-  <si>
-    <t>i9</t>
-  </si>
-  <si>
     <t>PUR_INV_ID</t>
   </si>
   <si>
@@ -171,12 +135,6 @@
     <t>Kanyin Face veneer</t>
   </si>
   <si>
-    <t>s4</t>
-  </si>
-  <si>
-    <t>i10</t>
-  </si>
-  <si>
     <t>Sinar Solo</t>
   </si>
   <si>
@@ -217,6 +175,48 @@
   </si>
   <si>
     <t>Taloja(COCHIN)</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>I4</t>
+  </si>
+  <si>
+    <t>I5</t>
+  </si>
+  <si>
+    <t>I6</t>
+  </si>
+  <si>
+    <t>I7</t>
+  </si>
+  <si>
+    <t>I8</t>
+  </si>
+  <si>
+    <t>I9</t>
+  </si>
+  <si>
+    <t>I10</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1074,7 +1074,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>24</v>
@@ -1083,19 +1083,19 @@
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>13</v>
@@ -1133,16 +1133,16 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
@@ -1151,10 +1151,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I2" s="3">
         <v>23800</v>
@@ -1192,16 +1192,16 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
@@ -1210,10 +1210,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I3" s="3">
         <v>23800</v>
@@ -1251,16 +1251,16 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>9</v>
@@ -1269,10 +1269,10 @@
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I4" s="3">
         <v>28000</v>
@@ -1310,16 +1310,16 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
@@ -1328,10 +1328,10 @@
         <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I5" s="3">
         <v>25200</v>
@@ -1369,16 +1369,16 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>9</v>
@@ -1387,10 +1387,10 @@
         <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I6" s="3">
         <v>26900</v>
@@ -1428,16 +1428,16 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>9</v>
@@ -1446,10 +1446,10 @@
         <v>5</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I7" s="3">
         <v>25200</v>
@@ -1487,16 +1487,16 @@
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>9</v>
@@ -1505,10 +1505,10 @@
         <v>6</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I8" s="3">
         <v>25200</v>
@@ -1546,16 +1546,16 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>10</v>
@@ -1564,10 +1564,10 @@
         <v>7</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I9" s="3">
         <v>104000</v>
@@ -1605,16 +1605,16 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>11</v>
@@ -1623,10 +1623,10 @@
         <v>12</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I10" s="3">
         <v>351800</v>
@@ -1664,25 +1664,25 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="I11" s="2">
         <v>109100</v>

</xml_diff>

<commit_message>
Fixed: now deducts items from specified PUR_INV_ID
</commit_message>
<xml_diff>
--- a/Invoice/pur_inv.xlsx
+++ b/Invoice/pur_inv.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
   <si>
     <t>f-001</t>
   </si>
@@ -217,6 +217,24 @@
   </si>
   <si>
     <t>S4</t>
+  </si>
+  <si>
+    <t>I11</t>
+  </si>
+  <si>
+    <t>SR1</t>
+  </si>
+  <si>
+    <t>Somayaji</t>
+  </si>
+  <si>
+    <t>28.11.2020</t>
+  </si>
+  <si>
+    <t>nill</t>
+  </si>
+  <si>
+    <t>INV-132</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1075,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1715,6 +1733,65 @@
         <v>1550</v>
       </c>
       <c r="S11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="2">
+        <v>300</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>350</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0</v>
+      </c>
+      <c r="S12" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>